<commit_message>
Updated the Status of file
The Requirements have been Approved
</commit_message>
<xml_diff>
--- a/Requirements_Analysis_VTLC_Version1.xlsx
+++ b/Requirements_Analysis_VTLC_Version1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Virtual-Traffic-Light-Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iastsoftware20-my.sharepoint.com/personal/shivarajkumar_iast-software_com/Documents/Documents/shivaraj/Assignments_Works/VersionControl/Virtual-Traffic-Light-Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E63437-2693-4D64-B3DF-06D4B5060B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A1E63437-2693-4D64-B3DF-06D4B5060B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52BAAAE-6F56-4985-8E70-B3E343E06F8F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,10 +169,10 @@
     <t>Keerthana</t>
   </si>
   <si>
-    <t>In Review</t>
-  </si>
-  <si>
     <t>Shivaraj Kumar, Prateeksha Jain</t>
+  </si>
+  <si>
+    <t>Approved</t>
   </si>
 </sst>
 </file>
@@ -271,18 +271,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,7 +591,7 @@
   <dimension ref="A2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,47 +602,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>